<commit_message>
updated part1c, now use part1cb3, part1c to be removed
</commit_message>
<xml_diff>
--- a/20200930_Assesment1d_LinearProgramming_DesignOp_EA.xlsx
+++ b/20200930_Assesment1d_LinearProgramming_DesignOp_EA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2326f21fcfb2723d/Projects/UoB 4th Year/Design Optimisation Project/Design Optimisation Skills/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ege\Documents\GitHub\Design-Optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2354" documentId="8_{39B704ED-7B1A-44F8-AECC-0D016EF61FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{967FB489-B43F-4C66-B656-7E77AA336AC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C8A5B8-376D-4203-8D10-25A9B31B50BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{8027FE10-1248-4DE6-B680-62825772498E}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Example!$C$9:$E$9</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Part 1'!$F$3</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Part 1'!$F$4</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Part 1'!$F$19:$H$19</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Part 1'!$L$21</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -58,7 +58,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Example!$I$9</definedName>
@@ -74,7 +74,7 @@
     <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Example!$I$6</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Example!$I$7</definedName>
@@ -82,7 +82,7 @@
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Part 1'!$K$3</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Part 1'!$K$4</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">integer</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Part 1'!$K$6</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Unit Profit, £</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Cost of Investment Location A</t>
+  </si>
+  <si>
+    <t>Cost of Investment Location B</t>
+  </si>
+  <si>
+    <t>Cost of Investment Location C</t>
   </si>
 </sst>
 </file>
@@ -464,7 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -484,6 +493,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -503,72 +513,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C05DC3C-36FB-4E58-8320-4E792DA2C36B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9372600" y="4381500"/>
-          <a:ext cx="6105525" cy="962025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -990,15 +934,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AE796E-3B81-450D-9202-E68979C155B3}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -1006,7 +950,8 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1041,7 +986,7 @@
       </c>
       <c r="F2" s="3">
         <f>SUMPRODUCT(B2:D2,Location_A_turbines)</f>
-        <v>4950</v>
+        <v>1750</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>17</v>
@@ -1270,7 +1215,7 @@
         <v>3063200</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E17" s="15" t="s">
         <v>33</v>
       </c>
@@ -1284,15 +1229,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="12">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="H18" s="11">
         <v>0</v>
@@ -1302,10 +1247,17 @@
       </c>
       <c r="J18" s="7">
         <f>SUMPRODUCT(Annual_Earnings_per_turbine_location_A,Location_A_turbines)</f>
-        <v>10503900</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+        <v>3639600</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="16">
+        <f>SUMPRODUCT(B10:D10,Location_A_turbines)</f>
+        <v>3494490</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E19" s="9" t="s">
         <v>18</v>
       </c>
@@ -1325,8 +1277,15 @@
         <f>SUMPRODUCT(Annual_Earnings_per_turbine_location_B,Location_B_turbines)</f>
         <v>49199430</v>
       </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="16">
+        <f>SUMPRODUCT(B11:D11,Location_A_turbines)</f>
+        <v>42352600</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E20" s="9" t="s">
         <v>19</v>
       </c>
@@ -1346,17 +1305,31 @@
         <f>SUMPRODUCT(Annual_Earnings_per_turbine_location_C,Location_C_turbines)</f>
         <v>4464000</v>
       </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="16">
+        <f>SUMPRODUCT(B12:D12,Location_A_turbines)</f>
+        <v>52815600</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="I21" s="7" t="s">
         <v>34</v>
       </c>
       <c r="J21" s="16">
         <f>SUM(J18:J20)</f>
-        <v>64167330</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+        <v>57303030</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="16">
+        <f>SUM(L18:L20)</f>
+        <v>98662690</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E24" s="15" t="s">
         <v>33</v>
       </c>
@@ -1364,44 +1337,45 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
       <c r="E25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="8">
-        <f>SUMPRODUCT(B7:D7,Location_A_turbines)-((SUMPRODUCT(B10:D10,Location_A_turbines)+(SUMPRODUCT(B13:D13,Location_A_turbines)))/((SUMPRODUCT(B10:D10,Location_A_turbines)+(SUMPRODUCT(B13:D13,Location_A_turbines)))))</f>
-        <v>210077999</v>
-      </c>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(B7:D7,Location_A_turbines)-((SUMPRODUCT(B10:D10,Location_A_turbines)+(SUMPRODUCT(B13:D13,Location_A_turbines)))/((SUMPRODUCT(B10:D10,Location_A_turbines)+(SUMPRODUCT(B13:D13,Location_A_turbines))))) -($K$6/3)</f>
+        <v>39458665.666666672</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
       <c r="E26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="8">
-        <f>SUMPRODUCT(B8:D8,Location_A_turbines)-((SUMPRODUCT(B11:D11,Location_A_turbines)+(SUMPRODUCT(B14:D14,Location_A_turbines)))/((SUMPRODUCT(B11:D11,Location_A_turbines)+(SUMPRODUCT(B14:D14,Location_A_turbines)))))</f>
-        <v>278097599</v>
-      </c>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(B8:D8,Location_A_turbines)-((SUMPRODUCT(B11:D11,Location_A_turbines)+(SUMPRODUCT(B14:D14,Location_A_turbines)))/((SUMPRODUCT(B11:D11,Location_A_turbines)+(SUMPRODUCT(B14:D14,Location_A_turbines))))) -($K$6/3)</f>
+        <v>64237265.666666672</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="8">
-        <f>SUMPRODUCT(B9:D9,Location_A_turbines)-((SUMPRODUCT(B12:D12,Location_A_turbines)+(SUMPRODUCT(B15:D15,Location_A_turbines)))/((SUMPRODUCT(B12:D12,Location_A_turbines)+(SUMPRODUCT(B15:D15,Location_A_turbines)))))</f>
-        <v>351053999</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(B9:D9,Location_A_turbines)-((SUMPRODUCT(B12:D12,Location_A_turbines)+(SUMPRODUCT(B15:D15,Location_A_turbines)))/((SUMPRODUCT(B12:D12,Location_A_turbines)+(SUMPRODUCT(B15:D15,Location_A_turbines))))) -($K$6/3)</f>
+        <v>88662165.666666672</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E28" s="15" t="s">
         <v>43</v>
       </c>
       <c r="F28" s="17">
         <f>SUM(F25:F27)</f>
-        <v>839229597</v>
+        <v>192358097</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the deliverables folder
</commit_message>
<xml_diff>
--- a/20200930_Assesment1d_LinearProgramming_DesignOp_EA.xlsx
+++ b/20200930_Assesment1d_LinearProgramming_DesignOp_EA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ege\Documents\GitHub\Design-Optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C8A5B8-376D-4203-8D10-25A9B31B50BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D66F8D-CEE8-4DF7-AF2E-30DF76882446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{8027FE10-1248-4DE6-B680-62825772498E}"/>
   </bookViews>
@@ -513,6 +513,133 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{269027EE-0130-49BC-ACEF-391980C7FE80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9715500" y="4572000"/>
+          <a:ext cx="3629025" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>386798</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6730A7B-1E05-4FD8-AA2B-B4949BD0CE75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9740348" y="5524500"/>
+          <a:ext cx="2358059" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AE796E-3B81-450D-9202-E68979C155B3}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,5 +1504,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>